<commit_message>
Adding some final changes
> Fixed build error in RecipeService.
> Updated sprint 4 backlog.
> Updated web wireframing.
</commit_message>
<xml_diff>
--- a/sprints/Sprint4/Sprint 4 Backlog Burndown Chart.xlsx
+++ b/sprints/Sprint4/Sprint 4 Backlog Burndown Chart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>Related User Story</t>
   </si>
@@ -236,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -250,15 +250,18 @@
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="5" fillId="3" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="5" fillId="4" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="5" fillId="5" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="5" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="5" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="5" fillId="6" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="5" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="5" fillId="5" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="5" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
@@ -329,11 +332,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1548348199"/>
-        <c:axId val="1683700115"/>
+        <c:axId val="1633781269"/>
+        <c:axId val="139160976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1548348199"/>
+        <c:axId val="1633781269"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -385,10 +388,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1683700115"/>
+        <c:crossAx val="139160976"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1683700115"/>
+        <c:axId val="139160976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -452,7 +455,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1548348199"/>
+        <c:crossAx val="1633781269"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -746,9 +749,15 @@
       <c r="C3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="D3" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="E3" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="6"/>
@@ -758,29 +767,31 @@
       <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>3.0</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>2.0</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="8">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="6"/>
       <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="7">
+        <v>3.0</v>
+      </c>
+      <c r="E5" s="8">
         <v>2.0</v>
       </c>
-      <c r="E5" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="F5" s="9">
+      <c r="F5" s="8">
         <v>0.0</v>
       </c>
     </row>
@@ -792,11 +803,13 @@
       <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9">
+      <c r="D6" s="7">
+        <v>3.0</v>
+      </c>
+      <c r="E6" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="F6" s="8">
         <v>2.0</v>
       </c>
     </row>
@@ -808,67 +821,83 @@
       <c r="C7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="D7" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="E7" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="6"/>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <v>2.0</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <v>1.0</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="8">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="6"/>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="7">
         <v>1.0</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9">
+      <c r="E9" s="8"/>
+      <c r="F9" s="8">
         <v>1.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="6"/>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+      <c r="C10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="7">
+        <v>3.0</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="6"/>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="E11" s="9">
+      <c r="D11" s="7">
+        <v>4.0</v>
+      </c>
+      <c r="E11" s="8">
         <v>1.0</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <v>0.0</v>
       </c>
     </row>
@@ -877,350 +906,372 @@
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="7">
         <v>1.0</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="8">
         <v>1.0</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="8">
         <v>0.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="6"/>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="7">
         <v>1.0</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="8">
         <v>1.0</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="8">
         <v>0.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="6"/>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="7">
         <v>0.1</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="8">
         <v>0.1</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="8">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="6"/>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="7">
         <v>0.1</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="8">
         <v>0.1</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="8">
         <v>0.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6"/>
-      <c r="B17" s="8"/>
+      <c r="B17" s="7"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="7">
         <v>0.1</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="8">
         <v>0.1</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="8">
         <v>0.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6"/>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="9">
+      <c r="D20" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="8">
         <v>1.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6"/>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+      <c r="D21" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="E21" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="F21" s="8">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="6"/>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="7">
+        <v>4.0</v>
+      </c>
+      <c r="E22" s="8">
         <v>2.0</v>
       </c>
-      <c r="E22" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="F22" s="9">
+      <c r="F22" s="8">
         <v>0.0</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="6"/>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="7">
         <v>2.0</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="9">
+      <c r="E23" s="11"/>
+      <c r="F23" s="8">
         <v>2.0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="6"/>
-      <c r="B24" s="8"/>
+      <c r="B24" s="7"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="7">
         <v>1.0</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="8">
         <v>1.0</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26" s="8">
         <v>0.0</v>
       </c>
     </row>
     <row r="27" ht="16.5" customHeight="1">
       <c r="A27" s="6"/>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="E27" s="8">
         <v>0.25</v>
       </c>
-      <c r="E27" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="F27" s="9">
+      <c r="F27" s="8">
         <v>0.0</v>
       </c>
     </row>
     <row r="28" ht="16.5" customHeight="1">
       <c r="A28" s="6"/>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D28" s="7">
         <v>0.5</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="9">
+      <c r="E28" s="11"/>
+      <c r="F28" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="6"/>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
+      <c r="D29" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="E29" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="F29" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="6"/>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="E30" s="8">
         <v>1.0</v>
       </c>
-      <c r="E30" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="F30" s="7">
+      <c r="F30" s="11">
         <v>0.0</v>
       </c>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="6"/>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D31" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="E31" s="11"/>
+      <c r="F31" s="8">
         <v>1.0</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="6"/>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D32" s="7">
         <v>0.5</v>
       </c>
-      <c r="E32" s="9">
+      <c r="E32" s="8">
         <v>0.5</v>
       </c>
-      <c r="F32" s="7"/>
+      <c r="F32" s="8">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="8"/>
+      <c r="A33" s="7"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12" t="s">
+      <c r="A36" s="13"/>
+      <c r="B36" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="13">
+      <c r="C36" s="13"/>
+      <c r="D36" s="14">
         <f t="shared" ref="D36:F36" si="1">SUM(D3:D35)</f>
-        <v>23.55</v>
-      </c>
-      <c r="E36" s="13">
+        <v>49.8</v>
+      </c>
+      <c r="E36" s="14">
         <f t="shared" si="1"/>
-        <v>13.05</v>
-      </c>
-      <c r="F36" s="13">
+        <v>26.05</v>
+      </c>
+      <c r="F36" s="14">
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>

</xml_diff>